<commit_message>
commit after long time
</commit_message>
<xml_diff>
--- a/TestRunnerBDD.xlsx
+++ b/TestRunnerBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DANISH\IdeaProjects\AutomationFramework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B290D03-032B-4246-BD68-B06C180B12FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F99D9A-93E1-4BCD-B711-E401FA6A0ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{8F340B59-7FB3-4D4C-A7C9-85DE4CD533C5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Feature file name</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Decision</t>
+  </si>
+  <si>
+    <t>@firstflow</t>
   </si>
 </sst>
 </file>
@@ -439,6 +442,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -471,13 +477,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9A2311-0142-4EDE-A320-9B82F6545D2E}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -487,7 +496,16 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>